<commit_message>
Remove tooltip when no longer needed.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dummy_data.xlsx
+++ b/DECS Excel Add-Ins/test files/dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6695A2-9819-4343-96AE-BD09FF569474}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6448AD0E-5644-43BC-A821-7319C951EC09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
     </r>
   </si>
   <si>
-    <t>`Date of Exam: 30 May 1979. Air temparature: 99.0 °F. air pressure: .`</t>
+    <t>`Date of Exam: 7-5-1975, 30 May 1979, Jan. 01, 1995 . Air temparature: 99.0 °F. air pressure: .`</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Handle multiple matches on same line.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dummy_data.xlsx
+++ b/DECS Excel Add-Ins/test files/dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6448AD0E-5644-43BC-A821-7319C951EC09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5257282E-D8D3-4278-80A8-3133C45DEB70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>`Date of Exam: 12/25/1999. Air temperature: 79.0 degF. Air pressure: 1013.2 mBar.`</t>
-  </si>
-  <si>
-    <t>`Date of Exam: 4-1-2023. Air pressure: 1234.5 mBar.'</t>
   </si>
   <si>
     <r>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>`Date of Exam: 7-5-1975, 30 May 1979, Jan. 01, 1995 . Air temparature: 99.0 °F. air pressure: .`</t>
+  </si>
+  <si>
+    <t>`Date of Exam: 4-1-2023, April 1st, 2023, May 2nd, 2023, June 3rd, 2023, July 4th, 2023. Air pressure: 1234.5 mBar.'</t>
   </si>
 </sst>
 </file>
@@ -446,12 +446,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>2354</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -501,7 +501,7 @@
         <v>3456</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -515,7 +515,7 @@
         <v>4567</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add left/right preference controls.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dummy_data.xlsx
+++ b/DECS Excel Add-Ins/test files/dummy_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8575E9-23E4-4548-A279-748AEDEC84D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE281C8-8C85-41E9-97D1-5A223D621DD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>REPORT</t>
-  </si>
-  <si>
-    <t>`Date of Exam: 12/25/1999. Air temperature: 79.0 degF. Air pressure: 1013.2 mBar.`</t>
   </si>
   <si>
     <r>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>`Date of Exam: 4-1-2023, 05-02-2024. April 1st, 2023, May 2nd, 2023, June 3rd, 2023, July 4th, 2023. Air pressure: 1234.5 mBar.'</t>
+  </si>
+  <si>
+    <t>`Date of Exam: 12/25/1999. Air temperature: 79.0 degF. Air pressure: 1013.2 mBar. Air temperature: 81.0 degF`</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>1234</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -490,7 +490,7 @@
         <v>2354</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -504,7 +504,7 @@
         <v>3456</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -518,7 +518,7 @@
         <v>4567</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -532,7 +532,7 @@
         <v>2354</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>